<commit_message>
Update excel test file and results
</commit_message>
<xml_diff>
--- a/tests/test_files/excel/pilot.xlsx
+++ b/tests/test_files/excel/pilot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1D8F6E-44EB-BA4C-B580-4F591F0F6866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E9D117-1D67-C24E-9A5A-8F5FC1EB86F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="500" windowWidth="41180" windowHeight="27240" firstSheet="20" activeTab="27" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="8320" yWindow="500" windowWidth="41180" windowHeight="27240" firstSheet="20" activeTab="28" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3257" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="1550">
   <si>
     <t>Screening</t>
   </si>
@@ -6834,6 +6834,15 @@
   <si>
     <t>@plannedAge/Range/@maxValue/Quantity/@value</t>
   </si>
+  <si>
+    <t>AMEND_1</t>
+  </si>
+  <si>
+    <t>The first amendment</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
 </sst>
 </file>
 
@@ -7195,16 +7204,16 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -13943,72 +13952,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A36B6E2-81ED-B543-A330-D9502D2DF96E}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="1" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>1495</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="I1" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="J1" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>1509</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>1496</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>1510</v>
       </c>
     </row>
@@ -15468,7 +15496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -15603,10 +15631,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666D5CD6-DF98-6447-9150-7AA4E8F8C9F3}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15615,7 +15643,7 @@
     <col min="7" max="7" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>216</v>
       </c>
@@ -15637,8 +15665,11 @@
       <c r="G1" s="16" t="s">
         <v>1489</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="16" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1490</v>
       </c>
@@ -21183,169 +21214,169 @@
       <c r="A1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="72" t="s">
         <v>520</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>1544</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>412</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>514</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>515</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="73" t="s">
         <v>516</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>430</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -21437,11 +21468,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
@@ -21451,6 +21477,11 @@
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21515,6 +21546,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -21715,15 +21755,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -21736,6 +21767,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21750,14 +21789,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>